<commit_message>
all possible runs added and cleaned up, changed naive Gap in TestLoop.gms
</commit_message>
<xml_diff>
--- a/Results/United/Omega01_10Iter_a_100Scen_HPC.xlsx
+++ b/Results/United/Omega01_10Iter_a_100Scen_HPC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\6.Semester\Bachelor-Arbeit\bachelor-thesis\Results\United\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E6745F-3B9E-42F7-B3FB-B7733BD22A32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802680A0-25A2-4EB5-B94B-D7F7FEDD19C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -281,8 +281,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -644,7 +647,7 @@
   <dimension ref="A1:Q121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -797,7 +800,7 @@
       <c r="M3">
         <v>4.9059499999999998</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <v>0.05</v>
       </c>
       <c r="P3" t="s">
@@ -2210,7 +2213,7 @@
       <c r="M33">
         <v>2.3719800000000002</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="1">
         <v>0.25</v>
       </c>
       <c r="P33" t="s">

</xml_diff>